<commit_message>
revisão código e atualização arquivo
</commit_message>
<xml_diff>
--- a/Planejamento Geral.xlsx
+++ b/Planejamento Geral.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" updateLinks="always" codeName="EstaPastaDeTrabalho"/>
-  <xr:revisionPtr revIDLastSave="2321" documentId="13_ncr:1_{8CB3FCBC-DACE-4BCA-A656-CE7D6185D885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB6BE95B-B973-413B-A946-C86BF8CDDC8D}"/>
+  <xr:revisionPtr revIDLastSave="2322" documentId="13_ncr:1_{8CB3FCBC-DACE-4BCA-A656-CE7D6185D885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{053AA7D2-2530-4681-BDFD-ACE7DDB1E707}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="363" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planejamento IED" sheetId="11" r:id="rId1"/>
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Embarques Vivenciais'!$A$76:$H$97</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Equipe!$A$1:$I$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planejamento IED'!$A$1:$E$1028</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planejamento IED'!$A$1:$E$1027</definedName>
     <definedName name="Hoje" localSheetId="3">TODAY()</definedName>
     <definedName name="Hoje" localSheetId="0">TODAY()</definedName>
     <definedName name="Início_da_tarefa" localSheetId="3">'3 Pessoas'!$E1</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="308">
   <si>
     <t>Nome</t>
   </si>
@@ -485,12 +485,6 @@
   </si>
   <si>
     <t>Folga alinhada</t>
-  </si>
-  <si>
-    <t>01/</t>
-  </si>
-  <si>
-    <t>Treinamento presencial no EDIHB</t>
   </si>
   <si>
     <t>RICARDO UEMA</t>
@@ -9106,8 +9100,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6AB63F5-01C4-4ED8-B3C5-D3AEB2DB48F3}" name="Tabela1" displayName="Tabela1" ref="A1:I1028" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54" dataCellStyle="Nome">
-  <autoFilter ref="A1:I1028" xr:uid="{D6AB63F5-01C4-4ED8-B3C5-D3AEB2DB48F3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6AB63F5-01C4-4ED8-B3C5-D3AEB2DB48F3}" name="Tabela1" displayName="Tabela1" ref="A1:I1027" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54" dataCellStyle="Nome">
+  <autoFilter ref="A1:I1027" xr:uid="{D6AB63F5-01C4-4ED8-B3C5-D3AEB2DB48F3}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C8A8658B-B54C-47E5-A350-3E4123B94A55}" name="Nome" dataDxfId="53" dataCellStyle="Nome"/>
     <tableColumn id="2" xr3:uid="{41F4E0E6-9B25-4120-B6CD-9E09A0162769}" name="Matrícula" dataDxfId="52" dataCellStyle="Nome">
@@ -9397,11 +9391,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L1028"/>
+  <dimension ref="A1:L1027"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G167" sqref="G167"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14728,44 +14722,43 @@
     </row>
     <row r="163" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="86" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="B163" s="105">
         <f>_xlfn.XLOOKUP(A163,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>9683150</v>
-      </c>
-      <c r="C163" s="90" t="s">
-        <v>144</v>
-      </c>
-      <c r="D163" s="106" t="e">
-        <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C163+E163-1,"")</f>
-        <v>#VALUE!</v>
+        <v>4612247</v>
+      </c>
+      <c r="C163" s="90">
+        <v>45875</v>
+      </c>
+      <c r="D163" s="106">
+        <v>45875</v>
       </c>
       <c r="E163" s="86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F163" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G163" s="98" t="s">
-        <v>145</v>
+      <c r="G163" s="133" t="s">
+        <v>85</v>
       </c>
       <c r="H163" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
-        <v>P80</v>
+        <v>A definir</v>
       </c>
       <c r="I163" s="39" t="str">
         <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
-        <v>Experiente</v>
+        <v>Novo</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="86" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B164" s="105">
         <f>_xlfn.XLOOKUP(A164,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>4612247</v>
+        <v>4612393</v>
       </c>
       <c r="C164" s="90">
         <v>45875</v>
@@ -14779,8 +14772,8 @@
       <c r="F164" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G164" s="133" t="s">
-        <v>85</v>
+      <c r="G164" s="98" t="s">
+        <v>122</v>
       </c>
       <c r="H164" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
@@ -14793,26 +14786,26 @@
     </row>
     <row r="165" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="86" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B165" s="105">
         <f>_xlfn.XLOOKUP(A165,Equipe!H:H,Equipe!B:B,"",0)</f>
         <v>4612393</v>
       </c>
       <c r="C165" s="90">
-        <v>45875</v>
+        <v>45887</v>
       </c>
       <c r="D165" s="106">
-        <v>45875</v>
+        <v>45891</v>
       </c>
       <c r="E165" s="86">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F165" s="86" t="s">
         <v>16</v>
       </c>
       <c r="G165" s="98" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H165" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
@@ -14825,17 +14818,17 @@
     </row>
     <row r="166" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="86" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B166" s="105">
         <f>_xlfn.XLOOKUP(A166,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>4612393</v>
+        <v>4612247</v>
       </c>
       <c r="C166" s="90">
-        <v>45887</v>
+        <v>45880</v>
       </c>
       <c r="D166" s="106">
-        <v>45891</v>
+        <v>45884</v>
       </c>
       <c r="E166" s="86">
         <v>5</v>
@@ -14861,22 +14854,23 @@
       </c>
       <c r="B167" s="105">
         <f>_xlfn.XLOOKUP(A167,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>4612247</v>
+        <v>4612228</v>
       </c>
       <c r="C167" s="90">
-        <v>45880</v>
+        <v>45877</v>
       </c>
       <c r="D167" s="106">
-        <v>45884</v>
+        <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C167+E167-1,"")</f>
+        <v>45877</v>
       </c>
       <c r="E167" s="86">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F167" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G167" s="98" t="s">
-        <v>123</v>
+      <c r="G167" s="134" t="s">
+        <v>122</v>
       </c>
       <c r="H167" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
@@ -14889,35 +14883,35 @@
     </row>
     <row r="168" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="86" t="s">
-        <v>148</v>
+        <v>36</v>
       </c>
       <c r="B168" s="105">
         <f>_xlfn.XLOOKUP(A168,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>4612228</v>
+        <v>9634222</v>
       </c>
       <c r="C168" s="90">
-        <v>45877</v>
+        <v>45881</v>
       </c>
       <c r="D168" s="106">
         <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C168+E168-1,"")</f>
-        <v>45877</v>
+        <v>45894</v>
       </c>
       <c r="E168" s="86">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F168" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="G168" s="134" t="s">
-        <v>122</v>
+        <v>11</v>
+      </c>
+      <c r="G168" s="98" t="s">
+        <v>99</v>
       </c>
       <c r="H168" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
-        <v>A definir</v>
+        <v>PBAC</v>
       </c>
       <c r="I168" s="39" t="str">
         <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
-        <v>Novo</v>
+        <v>Experiente</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14929,20 +14923,20 @@
         <v>9634222</v>
       </c>
       <c r="C169" s="90">
-        <v>45881</v>
+        <v>45895</v>
       </c>
       <c r="D169" s="106">
         <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C169+E169-1,"")</f>
-        <v>45894</v>
+        <v>45915</v>
       </c>
       <c r="E169" s="86">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F169" s="86" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G169" s="98" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="H169" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
@@ -14954,36 +14948,26 @@
       </c>
     </row>
     <row r="170" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="86" t="s">
-        <v>36</v>
-      </c>
+      <c r="A170" s="86"/>
       <c r="B170" s="105">
         <f>_xlfn.XLOOKUP(A170,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>9634222</v>
-      </c>
-      <c r="C170" s="90">
-        <v>45895</v>
-      </c>
-      <c r="D170" s="106">
+        <v>0</v>
+      </c>
+      <c r="C170" s="90"/>
+      <c r="D170" s="106" t="str">
         <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C170+E170-1,"")</f>
-        <v>45915</v>
-      </c>
-      <c r="E170" s="86">
-        <v>21</v>
-      </c>
-      <c r="F170" s="86" t="s">
-        <v>17</v>
-      </c>
-      <c r="G170" s="98" t="s">
-        <v>149</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E170" s="86"/>
+      <c r="F170" s="86"/>
+      <c r="G170" s="98"/>
       <c r="H170" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
-        <v>PBAC</v>
-      </c>
-      <c r="I170" s="39" t="str">
-        <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
-        <v>Experiente</v>
+        <v>ERRO</v>
+      </c>
+      <c r="I170" s="39" t="e">
+        <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17861,7 +17845,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="296" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="86"/>
       <c r="B296" s="105">
         <f>_xlfn.XLOOKUP(A296,Equipe!H:H,Equipe!B:B,"",0)</f>
@@ -34651,7 +34635,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="1026" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1026" spans="1:9" ht="1.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1026" s="86"/>
       <c r="B1026" s="105">
         <f>_xlfn.XLOOKUP(A1026,Equipe!H:H,Equipe!B:B,"",0)</f>
@@ -34674,47 +34658,24 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="1027" spans="1:9" ht="1.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1027" s="86"/>
-      <c r="B1027" s="105">
-        <f>_xlfn.XLOOKUP(A1027,Equipe!H:H,Equipe!B:B,"",0)</f>
-        <v>0</v>
-      </c>
-      <c r="C1027" s="90"/>
-      <c r="D1027" s="106" t="str">
+    <row r="1027" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1027" s="89"/>
+      <c r="B1027" s="89">
+        <v>4608</v>
+      </c>
+      <c r="C1027" s="91"/>
+      <c r="D1027" s="108" t="str">
         <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C1027+E1027-1,"")</f>
         <v/>
       </c>
-      <c r="E1027" s="86"/>
-      <c r="F1027" s="86"/>
-      <c r="G1027" s="98"/>
+      <c r="E1027" s="89"/>
+      <c r="F1027" s="89"/>
+      <c r="G1027" s="101"/>
       <c r="H1027" s="39" t="str">
         <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
         <v>ERRO</v>
       </c>
       <c r="I1027" s="39" t="e">
-        <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1028" s="89"/>
-      <c r="B1028" s="89">
-        <v>4608</v>
-      </c>
-      <c r="C1028" s="91"/>
-      <c r="D1028" s="108" t="str">
-        <f>IF(Tabela1[[#This Row],[Início]]&lt;&gt;"",C1028+E1028-1,"")</f>
-        <v/>
-      </c>
-      <c r="E1028" s="89"/>
-      <c r="F1028" s="89"/>
-      <c r="G1028" s="101"/>
-      <c r="H1028" s="39" t="str">
-        <f>_xlfn.XLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:B,Equipe!E:E,"ERRO",0)</f>
-        <v>ERRO</v>
-      </c>
-      <c r="I1028" s="39" t="e">
         <f>VLOOKUP(Tabela1[[#This Row],[Matrícula]],Equipe!B:F,5,0)</f>
         <v>#N/A</v>
       </c>
@@ -34724,7 +34685,7 @@
     <mergeCell ref="L5:L8"/>
   </mergeCells>
   <phoneticPr fontId="29" type="noConversion"/>
-  <conditionalFormatting sqref="A1:XFD1 C2:XFD3 K2:K6 A2:B33 L4:XFD4 E4:J61 C4:D67 L9:XFD1048576 K10:K1048576 A34:A53 B34:B63 A55:A63 E62:I72 J62:J1048576 A64:B67 A68:C69 D68:D72 A69:B71 A72:C72 A73:I84 A85:B86 D85:I86 A87:I107 A108:B108 D108:I108 A109:I116 A117:F117 H117:I117 A118:I147 A148:B148 D148:I148 A149:I163 A164:F164 H164:I164 A165:I167 A168:F168 H168:I168 A169:I1048576">
+  <conditionalFormatting sqref="A1:XFD1 C2:XFD3 K2:K6 A2:B33 L4:XFD4 E4:J61 C4:D67 A34:A53 B34:B63 A55:A63 E62:I72 A64:B67 A68:C69 D68:D72 A69:B71 A72:C72 A73:I84 A85:B86 D85:I86 A87:I107 A108:B108 D108:I108 A109:I116 A117:F117 H117:I117 A118:I147 A148:B148 D148:I148 A149:I162 A163:F163 H163:I163 A164:I166 A167:F167 H167:I167 A168:I1048576 L9:XFD1048576 K10:K1048576 J62:J1048576">
     <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
       <formula>"ESTALEIRO"</formula>
     </cfRule>
@@ -34755,10 +34716,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1028:F1128" xr:uid="{FE92769D-A30C-45A3-B10C-426BB3355AD8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1027:F1127" xr:uid="{FE92769D-A30C-45A3-B10C-426BB3355AD8}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1027" xr:uid="{156E15E9-23E7-431B-9B12-A26E3B0A7469}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1026" xr:uid="{156E15E9-23E7-431B-9B12-A26E3B0A7469}">
       <formula1>$K$2:$K$11</formula1>
     </dataValidation>
   </dataValidations>
@@ -34782,7 +34743,7 @@
           <x14:formula1>
             <xm:f>Equipe!$H$2:$H$131</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1027</xm:sqref>
+          <xm:sqref>A2:A1026</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -34795,9 +34756,9 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34815,1379 +34776,1379 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="113" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B1" s="114" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="114" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="115" t="s">
         <v>151</v>
-      </c>
-      <c r="D1" s="114" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="115" t="s">
-        <v>153</v>
       </c>
       <c r="F1" s="115" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="115" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H1" s="115" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="84" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="116">
         <v>4612171</v>
       </c>
       <c r="C2" s="116" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="118" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="117" t="s">
+      <c r="F2" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="118" t="s">
+      <c r="G2" s="119" t="s">
         <v>159</v>
-      </c>
-      <c r="F2" s="118" t="s">
-        <v>160</v>
-      </c>
-      <c r="G2" s="119" t="s">
-        <v>161</v>
       </c>
       <c r="H2" s="118" t="s">
         <v>118</v>
       </c>
       <c r="I2" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H27)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H27)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="110">
         <v>4612050</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="112" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="112" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="112" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="112" t="s">
-        <v>160</v>
-      </c>
       <c r="G3" s="120" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H3" s="112" t="s">
         <v>112</v>
       </c>
       <c r="I3" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H19)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H19)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="116">
         <v>4612140</v>
       </c>
       <c r="C4" s="116" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G4" s="119" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H4" s="118" t="s">
         <v>110</v>
       </c>
       <c r="I4" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H24)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H24)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" s="110">
         <v>9842940</v>
       </c>
       <c r="C5" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" s="120" t="s">
         <v>166</v>
-      </c>
-      <c r="D5" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" s="112" t="s">
-        <v>167</v>
-      </c>
-      <c r="F5" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="G5" s="120" t="s">
-        <v>168</v>
       </c>
       <c r="H5" s="112" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H25)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H25)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" s="110">
         <v>4608544</v>
       </c>
       <c r="C6" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="112" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="120" t="s">
         <v>169</v>
-      </c>
-      <c r="D6" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="112" t="s">
-        <v>170</v>
-      </c>
-      <c r="F6" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="G6" s="120" t="s">
-        <v>171</v>
       </c>
       <c r="H6" s="112" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H5)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H5)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="121" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B7" s="110">
         <v>4608559</v>
       </c>
       <c r="C7" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="123" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="123" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="124" t="s">
         <v>172</v>
-      </c>
-      <c r="D7" s="122" t="s">
-        <v>158</v>
-      </c>
-      <c r="E7" s="123" t="s">
-        <v>173</v>
-      </c>
-      <c r="F7" s="123" t="s">
-        <v>160</v>
-      </c>
-      <c r="G7" s="124" t="s">
-        <v>174</v>
       </c>
       <c r="H7" s="123" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="85" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="121" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8" s="110">
         <v>4606246</v>
       </c>
       <c r="C8" s="110" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="122" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="123" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="122" t="s">
+      <c r="F8" s="123" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="124" t="s">
         <v>177</v>
-      </c>
-      <c r="E8" s="123" t="s">
-        <v>178</v>
-      </c>
-      <c r="F8" s="123" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="124" t="s">
-        <v>179</v>
       </c>
       <c r="H8" s="123" t="s">
         <v>70</v>
       </c>
       <c r="I8" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H4)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H4)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B9" s="116">
         <v>9886449</v>
       </c>
       <c r="C9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="125" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="126" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" s="126" t="s">
+        <v>180</v>
+      </c>
+      <c r="G9" s="127" t="s">
         <v>181</v>
-      </c>
-      <c r="D9" s="125" t="s">
-        <v>158</v>
-      </c>
-      <c r="E9" s="126" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" s="126" t="s">
-        <v>182</v>
-      </c>
-      <c r="G9" s="127" t="s">
-        <v>183</v>
       </c>
       <c r="H9" s="126" t="s">
         <v>54</v>
       </c>
       <c r="I9" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H9)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H9)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="110">
         <v>4608721</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D10" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="123" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="123" t="s">
-        <v>167</v>
-      </c>
-      <c r="F10" s="123" t="s">
-        <v>160</v>
-      </c>
       <c r="G10" s="124" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H10" s="123" t="s">
         <v>30</v>
       </c>
       <c r="I10" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H8)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H8)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B11" s="116">
         <v>1385894</v>
       </c>
       <c r="C11" s="116" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D11" s="125" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E11" s="126" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" s="126" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G11" s="127" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H11" s="126" t="s">
         <v>32</v>
       </c>
       <c r="I11" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H20)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H20)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B12" s="110">
         <v>4608685</v>
       </c>
       <c r="C12" s="110" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D12" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" s="112" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="112" t="s">
-        <v>167</v>
-      </c>
-      <c r="F12" s="112" t="s">
-        <v>160</v>
-      </c>
       <c r="G12" s="120" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H12" s="112" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H3)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H3)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B13" s="116">
         <v>4608474</v>
       </c>
       <c r="C13" s="116" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D13" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="118" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="F13" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G13" s="119" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H13" s="118" t="s">
         <v>28</v>
       </c>
       <c r="I13" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H15)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H15)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B14" s="110">
         <v>1386344</v>
       </c>
       <c r="C14" s="110" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="112" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="112" t="s">
+        <v>180</v>
+      </c>
+      <c r="G14" s="120" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14" s="112" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="E14" s="112" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" s="112" t="s">
-        <v>182</v>
-      </c>
-      <c r="G14" s="120" t="s">
-        <v>193</v>
-      </c>
-      <c r="H14" s="112" t="s">
-        <v>194</v>
-      </c>
       <c r="I14" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H23)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H23)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B15" s="128">
         <v>4608684</v>
       </c>
       <c r="C15" s="116" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D15" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="118" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G15" s="119" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H15" s="118" t="s">
         <v>52</v>
       </c>
       <c r="I15" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H11)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H11)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B16" s="116">
         <v>4608411</v>
       </c>
       <c r="C16" s="116" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D16" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="118" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="126" t="s">
         <v>158</v>
       </c>
-      <c r="E16" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="F16" s="126" t="s">
-        <v>160</v>
-      </c>
       <c r="G16" s="127" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H16" s="126" t="s">
         <v>46</v>
       </c>
       <c r="I16" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H14)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H14)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B17" s="110">
         <v>9634180</v>
       </c>
       <c r="C17" s="110" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="123" t="s">
+        <v>171</v>
+      </c>
+      <c r="F17" s="123" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="124" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="123" t="s">
         <v>199</v>
       </c>
-      <c r="D17" s="122" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="123" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" s="123" t="s">
-        <v>182</v>
-      </c>
-      <c r="G17" s="124" t="s">
-        <v>200</v>
-      </c>
-      <c r="H17" s="123" t="s">
-        <v>201</v>
-      </c>
       <c r="I17" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H16)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H16)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B18" s="129">
         <v>4606308</v>
       </c>
       <c r="C18" s="116" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="125" t="s">
+        <v>175</v>
+      </c>
+      <c r="E18" s="126" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="126" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" s="127" t="s">
+        <v>201</v>
+      </c>
+      <c r="H18" s="118" t="s">
         <v>202</v>
       </c>
-      <c r="D18" s="125" t="s">
-        <v>177</v>
-      </c>
-      <c r="E18" s="126" t="s">
-        <v>178</v>
-      </c>
-      <c r="F18" s="126" t="s">
-        <v>160</v>
-      </c>
-      <c r="G18" s="127" t="s">
-        <v>203</v>
-      </c>
-      <c r="H18" s="118" t="s">
-        <v>204</v>
-      </c>
       <c r="I18" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H26)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H26)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B19" s="110">
         <v>9634222</v>
       </c>
       <c r="C19" s="110" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D19" s="122" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E19" s="123" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F19" s="112" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G19" s="124" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H19" s="123" t="s">
         <v>36</v>
       </c>
       <c r="I19" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H31)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H31)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B20" s="116">
         <v>229316</v>
       </c>
       <c r="C20" s="116" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D20" s="125" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E20" s="126" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F20" s="118" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G20" s="127" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H20" s="126" t="s">
         <v>124</v>
       </c>
       <c r="I20" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H2)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H2)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B21" s="110">
         <v>4612243</v>
       </c>
       <c r="C21" s="110" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D21" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="123" t="s">
+        <v>157</v>
+      </c>
+      <c r="F21" s="112" t="s">
         <v>158</v>
       </c>
-      <c r="E21" s="123" t="s">
-        <v>159</v>
-      </c>
-      <c r="F21" s="112" t="s">
-        <v>160</v>
-      </c>
       <c r="G21" s="124" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H21" s="123" t="s">
         <v>120</v>
       </c>
       <c r="I21" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H41)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H41)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B22" s="116">
         <v>4612389</v>
       </c>
       <c r="C22" s="116" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D22" s="125" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="126" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="126" t="s">
-        <v>159</v>
-      </c>
-      <c r="F22" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G22" s="119" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H22" s="118" t="s">
         <v>116</v>
       </c>
       <c r="I22" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H42)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H42)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B23" s="110">
         <v>4612192</v>
       </c>
       <c r="C23" s="110" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D23" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="E23" s="123" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="123" t="s">
-        <v>159</v>
-      </c>
-      <c r="F23" s="123" t="s">
-        <v>160</v>
-      </c>
       <c r="G23" s="124" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H23" s="123" t="s">
         <v>114</v>
       </c>
       <c r="I23" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H43)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H43)&gt;0,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B24" s="116">
         <v>4612393</v>
       </c>
       <c r="C24" s="116" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D24" s="125" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="126" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E24" s="126" t="s">
-        <v>159</v>
-      </c>
-      <c r="F24" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G24" s="127" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H24" s="126" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I24" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H44)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H44)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B25" s="110">
         <v>4612228</v>
       </c>
       <c r="C25" s="110" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D25" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E25" s="112" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" s="112" t="s">
         <v>158</v>
       </c>
-      <c r="E25" s="112" t="s">
-        <v>159</v>
-      </c>
-      <c r="F25" s="112" t="s">
-        <v>160</v>
-      </c>
       <c r="G25" s="120" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H25" s="112" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I25" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H45)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H45)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" s="116">
         <v>4612247</v>
       </c>
       <c r="C26" s="116" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D26" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G26" s="119" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H26" s="118" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I26" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H46)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H46)&gt;0,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B27" s="116">
         <v>9762281</v>
       </c>
       <c r="C27" s="116" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="118" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="127" t="s">
+        <v>221</v>
+      </c>
+      <c r="H27" s="126" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="117" t="s">
-        <v>158</v>
-      </c>
-      <c r="E27" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="F27" s="118" t="s">
-        <v>182</v>
-      </c>
-      <c r="G27" s="127" t="s">
-        <v>223</v>
-      </c>
-      <c r="H27" s="126" t="s">
-        <v>224</v>
-      </c>
       <c r="I27" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H6)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H6)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B28" s="110">
         <v>9683150</v>
       </c>
       <c r="C28" s="110" t="s">
+        <v>223</v>
+      </c>
+      <c r="D28" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="112" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="112" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="124" t="s">
+        <v>224</v>
+      </c>
+      <c r="H28" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="E28" s="112" t="s">
-        <v>167</v>
-      </c>
-      <c r="F28" s="112" t="s">
-        <v>182</v>
-      </c>
-      <c r="G28" s="124" t="s">
-        <v>226</v>
-      </c>
-      <c r="H28" s="123" t="s">
-        <v>227</v>
-      </c>
       <c r="I28" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H30)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H30)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B29" s="116">
         <v>2440812</v>
       </c>
       <c r="C29" s="116" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="117" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="126" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="118" t="s">
+        <v>180</v>
+      </c>
+      <c r="G29" s="127" t="s">
         <v>228</v>
-      </c>
-      <c r="D29" s="117" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" s="126" t="s">
-        <v>167</v>
-      </c>
-      <c r="F29" s="118" t="s">
-        <v>182</v>
-      </c>
-      <c r="G29" s="127" t="s">
-        <v>230</v>
       </c>
       <c r="H29" s="126" t="s">
         <v>65</v>
       </c>
       <c r="I29" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H28)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H28)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B30" s="110">
         <v>1381625</v>
       </c>
       <c r="C30" s="110" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D30" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E30" s="123" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F30" s="112" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G30" s="124" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H30" s="123" t="s">
         <v>38</v>
       </c>
       <c r="I30" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H12)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H12)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B31" s="116">
         <v>4608389</v>
       </c>
       <c r="C31" s="116" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D31" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E31" s="126" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="126" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="118" t="s">
-        <v>160</v>
-      </c>
       <c r="G31" s="127" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H31" s="126" t="s">
         <v>44</v>
       </c>
       <c r="I31" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H13)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H13)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B32" s="110">
         <v>9612082</v>
       </c>
       <c r="C32" s="110" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D32" s="110" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E32" s="80" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F32" s="80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G32" s="82" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H32" s="80" t="s">
         <v>58</v>
       </c>
       <c r="I32" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H7)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H7)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B33" s="116">
         <v>9618720</v>
       </c>
       <c r="C33" s="116" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D33" s="116" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E33" s="81" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F33" s="118" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G33" s="83" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H33" s="81" t="s">
         <v>56</v>
       </c>
       <c r="I33" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H22)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H22)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B34" s="110">
         <v>9724817</v>
       </c>
       <c r="C34" s="110" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D34" s="110" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E34" s="80" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F34" s="112" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G34" s="82" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H34" s="80" t="s">
         <v>34</v>
       </c>
       <c r="I34" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H10)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H10)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B35" s="116">
         <v>2460800</v>
       </c>
       <c r="C35" s="116" t="s">
+        <v>239</v>
+      </c>
+      <c r="D35" s="117" t="s">
+        <v>227</v>
+      </c>
+      <c r="E35" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="F35" s="81" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" s="83" t="s">
+        <v>240</v>
+      </c>
+      <c r="H35" s="81" t="s">
         <v>241</v>
       </c>
-      <c r="D35" s="117" t="s">
-        <v>229</v>
-      </c>
-      <c r="E35" s="81" t="s">
-        <v>170</v>
-      </c>
-      <c r="F35" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="G35" s="83" t="s">
-        <v>242</v>
-      </c>
-      <c r="H35" s="81" t="s">
-        <v>243</v>
-      </c>
       <c r="I35" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H29)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H29)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B36" s="116">
         <v>4608780</v>
       </c>
       <c r="C36" s="116" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D36" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="E36" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="F36" s="81" t="s">
-        <v>160</v>
-      </c>
       <c r="G36" s="83" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H36" s="81" t="s">
         <v>42</v>
       </c>
       <c r="I36" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H21)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H21)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B37" s="110">
         <v>2475130</v>
       </c>
       <c r="C37" s="110" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D37" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E37" s="80" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F37" s="80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G37" s="82" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H37" s="80" t="s">
         <v>90</v>
       </c>
       <c r="I37" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H18)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H18)&gt;0,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B38" s="116">
         <v>2477135</v>
       </c>
       <c r="C38" s="116" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D38" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E38" s="81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F38" s="81" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G38" s="83" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H38" s="81" t="s">
         <v>51</v>
       </c>
       <c r="I38" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H17)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H17)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B39" s="110">
         <v>2493288</v>
       </c>
       <c r="C39" s="110" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D39" s="111" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E39" s="80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F39" s="80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G39" s="82" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H39" s="80" t="s">
         <v>21</v>
       </c>
       <c r="I39" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H32)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H32)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B40" s="116">
         <v>214272</v>
       </c>
       <c r="C40" s="116" t="s">
+        <v>250</v>
+      </c>
+      <c r="D40" s="116" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="81" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="83" t="s">
+        <v>251</v>
+      </c>
+      <c r="H40" s="81" t="s">
         <v>252</v>
       </c>
-      <c r="D40" s="116" t="s">
-        <v>177</v>
-      </c>
-      <c r="E40" s="81" t="s">
-        <v>178</v>
-      </c>
-      <c r="F40" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="G40" s="83" t="s">
-        <v>253</v>
-      </c>
-      <c r="H40" s="81" t="s">
-        <v>254</v>
-      </c>
       <c r="I40" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H34)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H34)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B41" s="110">
         <v>4606694</v>
       </c>
       <c r="C41" s="110" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D41" s="111" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E41" s="80" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G41" s="82" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H41" s="80" t="s">
         <v>48</v>
       </c>
       <c r="I41" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H35)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H35)&gt;0,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B42" s="116">
         <v>2430855</v>
       </c>
       <c r="C42" s="116" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D42" s="117" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E42" s="81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F42" s="81" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G42" s="83" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H42" s="81" t="s">
         <v>23</v>
       </c>
       <c r="I42" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H36)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H36)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B43" s="110">
         <v>4604625</v>
       </c>
       <c r="C43" s="110" t="s">
+        <v>257</v>
+      </c>
+      <c r="D43" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="E43" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="F43" s="80" t="s">
+        <v>158</v>
+      </c>
+      <c r="G43" s="82" t="s">
         <v>259</v>
       </c>
-      <c r="D43" s="111" t="s">
+      <c r="H43" s="80" t="s">
         <v>260</v>
       </c>
-      <c r="E43" s="80" t="s">
-        <v>178</v>
-      </c>
-      <c r="F43" s="80" t="s">
-        <v>160</v>
-      </c>
-      <c r="G43" s="82" t="s">
-        <v>261</v>
-      </c>
-      <c r="H43" s="80" t="s">
-        <v>262</v>
-      </c>
       <c r="I43" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H37)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H37)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B44" s="116">
         <v>4612098</v>
       </c>
       <c r="C44" s="116" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D44" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="81" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="81" t="s">
-        <v>159</v>
-      </c>
-      <c r="F44" s="81" t="s">
-        <v>160</v>
-      </c>
       <c r="G44" s="83" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H44" s="81" t="s">
         <v>106</v>
       </c>
       <c r="I44" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H38)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H38)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B45" s="110">
         <v>4612126</v>
       </c>
       <c r="C45" s="110" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D45" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="80" t="s">
+        <v>157</v>
+      </c>
+      <c r="F45" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="80" t="s">
-        <v>159</v>
-      </c>
-      <c r="F45" s="80" t="s">
-        <v>160</v>
-      </c>
       <c r="G45" s="82" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H45" s="80" t="s">
         <v>130</v>
       </c>
       <c r="I45" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H39)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H39)&gt;0,"X","")</f>
         <v>X</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B46" s="116">
         <v>2550195</v>
       </c>
       <c r="C46" s="116" t="s">
+        <v>265</v>
+      </c>
+      <c r="D46" s="117" t="s">
+        <v>227</v>
+      </c>
+      <c r="E46" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="F46" s="81" t="s">
+        <v>180</v>
+      </c>
+      <c r="G46" s="83" t="s">
+        <v>266</v>
+      </c>
+      <c r="H46" s="81" t="s">
         <v>267</v>
       </c>
-      <c r="D46" s="117" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="F46" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="G46" s="83" t="s">
-        <v>268</v>
-      </c>
-      <c r="H46" s="81" t="s">
-        <v>269</v>
-      </c>
       <c r="I46" s="85" t="str">
-        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1028,Equipe!H40)&gt;0,"X","")</f>
+        <f>IF(COUNTIF('Planejamento IED'!$A$2:$A$1027,Equipe!H40)&gt;0,"X","")</f>
         <v/>
       </c>
     </row>
@@ -36357,25 +36318,25 @@
     <row r="1" spans="2:35" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:35" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="141" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C2" s="142"/>
       <c r="D2" s="142"/>
       <c r="E2" s="142"/>
       <c r="G2" s="137" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H2" s="137"/>
       <c r="I2" s="137"/>
       <c r="J2" s="137"/>
       <c r="L2" s="138" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M2" s="139"/>
       <c r="N2" s="139"/>
       <c r="O2" s="140"/>
       <c r="Q2" s="138" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="R2" s="139"/>
       <c r="S2" s="139"/>
@@ -36383,52 +36344,52 @@
     </row>
     <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" s="132" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="132" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="132" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="132" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="132" t="s">
-        <v>271</v>
-      </c>
-      <c r="D3" s="132" t="s">
+      <c r="G3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="H3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="I3" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="J3" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="E3" s="132" t="s">
-        <v>273</v>
-      </c>
-      <c r="G3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="H3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="I3" s="103" t="s">
+      <c r="L3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="M3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="N3" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="O3" s="85" t="s">
         <v>272</v>
       </c>
-      <c r="J3" s="85" t="s">
-        <v>274</v>
-      </c>
-      <c r="L3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="M3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="N3" s="103" t="s">
+      <c r="Q3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="R3" s="103" t="s">
+        <v>269</v>
+      </c>
+      <c r="S3" s="103" t="s">
+        <v>270</v>
+      </c>
+      <c r="T3" s="85" t="s">
         <v>272</v>
-      </c>
-      <c r="O3" s="85" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="R3" s="103" t="s">
-        <v>271</v>
-      </c>
-      <c r="S3" s="103" t="s">
-        <v>272</v>
-      </c>
-      <c r="T3" s="85" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="4" spans="2:35" x14ac:dyDescent="0.25">
@@ -37051,7 +37012,7 @@
         <v>9</v>
       </c>
       <c r="AI13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="2:35" x14ac:dyDescent="0.25">
@@ -38296,47 +38257,47 @@
     </row>
     <row r="76" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="113" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B76" s="114" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="114" t="s">
+        <v>149</v>
+      </c>
+      <c r="D76" s="114" t="s">
+        <v>150</v>
+      </c>
+      <c r="E76" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="D76" s="114" t="s">
-        <v>152</v>
-      </c>
-      <c r="E76" s="115" t="s">
-        <v>153</v>
-      </c>
       <c r="F76" s="115" t="s">
         <v>0</v>
       </c>
       <c r="G76" s="115" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H76" s="115" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S76"/>
       <c r="T76"/>
     </row>
     <row r="77" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B77" s="116">
         <v>4612171</v>
       </c>
       <c r="C77" s="116" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" s="117" t="s">
+        <v>156</v>
+      </c>
+      <c r="E77" s="118" t="s">
         <v>157</v>
-      </c>
-      <c r="D77" s="117" t="s">
-        <v>158</v>
-      </c>
-      <c r="E77" s="118" t="s">
-        <v>159</v>
       </c>
       <c r="F77" s="118" t="s">
         <v>118</v>
@@ -38354,19 +38315,19 @@
     </row>
     <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B78" s="110">
         <v>4612050</v>
       </c>
       <c r="C78" s="110" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D78" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E78" s="112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F78" s="112" t="s">
         <v>112</v>
@@ -38384,19 +38345,19 @@
     </row>
     <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="116">
         <v>4612140</v>
       </c>
       <c r="C79" s="116" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D79" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E79" s="118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F79" s="118" t="s">
         <v>110</v>
@@ -38414,19 +38375,19 @@
     </row>
     <row r="80" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B80" s="110">
         <v>4612243</v>
       </c>
       <c r="C80" s="110" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D80" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E80" s="112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F80" s="112" t="s">
         <v>120</v>
@@ -38444,19 +38405,19 @@
     </row>
     <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B81" s="116">
         <v>4612389</v>
       </c>
       <c r="C81" s="116" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D81" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E81" s="118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F81" s="118" t="s">
         <v>116</v>
@@ -38474,19 +38435,19 @@
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B82" s="110">
         <v>4612192</v>
       </c>
       <c r="C82" s="110" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D82" s="122" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E82" s="123" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F82" s="123" t="s">
         <v>114</v>
@@ -38504,22 +38465,22 @@
     </row>
     <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B83" s="116">
         <v>4612393</v>
       </c>
       <c r="C83" s="116" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D83" s="125" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E83" s="126" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F83" s="126" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G83" s="118">
         <f ca="1">COUNTIFS('Planejamento IED'!A:A,'Embarques Vivenciais'!F83,'Planejamento IED'!F:F,"Embarque",'Planejamento IED'!D:D,"&lt;="&amp;TODAY())</f>
@@ -38534,22 +38495,22 @@
     </row>
     <row r="84" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B84" s="110">
         <v>4612228</v>
       </c>
       <c r="C84" s="110" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D84" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E84" s="112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F84" s="112" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G84" s="118">
         <f ca="1">COUNTIFS('Planejamento IED'!A:A,'Embarques Vivenciais'!F84,'Planejamento IED'!F:F,"Embarque",'Planejamento IED'!D:D,"&lt;="&amp;TODAY())</f>
@@ -38564,22 +38525,22 @@
     </row>
     <row r="85" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="121" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B85" s="116">
         <v>4612247</v>
       </c>
       <c r="C85" s="116" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D85" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E85" s="118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F85" s="118" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G85" s="118">
         <f ca="1">COUNTIFS('Planejamento IED'!A:A,'Embarques Vivenciais'!F85,'Planejamento IED'!F:F,"Embarque",'Planejamento IED'!D:D,"&lt;="&amp;TODAY())</f>
@@ -38594,19 +38555,19 @@
     </row>
     <row r="86" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B86" s="116">
         <v>4612098</v>
       </c>
       <c r="C86" s="116" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D86" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E86" s="118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F86" s="118" t="s">
         <v>106</v>
@@ -38624,19 +38585,19 @@
     </row>
     <row r="87" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="121" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B87" s="110">
         <v>4612126</v>
       </c>
       <c r="C87" s="110" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D87" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E87" s="112" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F87" s="123" t="s">
         <v>130</v>
@@ -38654,19 +38615,19 @@
     </row>
     <row r="88" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B88" s="110">
         <v>9842940</v>
       </c>
       <c r="C88" s="110" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D88" s="122" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E88" s="123" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F88" s="123" t="s">
         <v>31</v>
@@ -38684,19 +38645,19 @@
     </row>
     <row r="89" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B89" s="110">
         <v>4608721</v>
       </c>
       <c r="C89" s="110" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D89" s="122" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E89" s="123" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F89" s="112" t="s">
         <v>30</v>
@@ -38714,19 +38675,19 @@
     </row>
     <row r="90" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B90" s="110">
         <v>4608685</v>
       </c>
       <c r="C90" s="110" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D90" s="122" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E90" s="123" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F90" s="123" t="s">
         <v>19</v>
@@ -38744,19 +38705,19 @@
     </row>
     <row r="91" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B91" s="116">
         <v>4608389</v>
       </c>
       <c r="C91" s="116" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D91" s="125" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E91" s="126" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F91" s="126" t="s">
         <v>44</v>
@@ -38774,19 +38735,19 @@
     </row>
     <row r="92" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B92" s="110">
         <v>4608544</v>
       </c>
       <c r="C92" s="110" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D92" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E92" s="112" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F92" s="112" t="s">
         <v>10</v>
@@ -38804,19 +38765,19 @@
     </row>
     <row r="93" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B93" s="116">
         <v>4608474</v>
       </c>
       <c r="C93" s="116" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D93" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E93" s="118" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F93" s="118" t="s">
         <v>28</v>
@@ -38834,19 +38795,19 @@
     </row>
     <row r="94" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B94" s="128">
         <v>4608684</v>
       </c>
       <c r="C94" s="116" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D94" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E94" s="126" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F94" s="126" t="s">
         <v>52</v>
@@ -38864,19 +38825,19 @@
     </row>
     <row r="95" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="79" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B95" s="110">
         <v>4608559</v>
       </c>
       <c r="C95" s="110" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D95" s="111" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E95" s="80" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F95" s="80" t="s">
         <v>14</v>
@@ -38894,19 +38855,19 @@
     </row>
     <row r="96" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B96" s="116">
         <v>4608411</v>
       </c>
       <c r="C96" s="116" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D96" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E96" s="81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F96" s="81" t="s">
         <v>46</v>
@@ -38924,19 +38885,19 @@
     </row>
     <row r="97" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B97" s="116">
         <v>4608780</v>
       </c>
       <c r="C97" s="116" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D97" s="117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E97" s="81" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F97" s="81" t="s">
         <v>42</v>
@@ -39067,10 +39028,10 @@
   <sheetData>
     <row r="1" spans="1:239" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -39078,31 +39039,31 @@
       <c r="F1" s="31"/>
       <c r="H1" s="2"/>
       <c r="I1" s="50" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:239" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I2" s="51"/>
     </row>
     <row r="3" spans="1:239" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C3" s="69">
         <f>Início_do_projeto+120</f>
         <v>46051</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E3" s="146">
         <v>45931</v>
@@ -39112,10 +39073,10 @@
     </row>
     <row r="4" spans="1:239" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C4" s="147" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D4" s="148"/>
       <c r="E4" s="7">
@@ -39454,7 +39415,7 @@
     </row>
     <row r="5" spans="1:239" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
@@ -40389,22 +40350,22 @@
     </row>
     <row r="6" spans="1:239" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>291</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>293</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
@@ -41337,7 +41298,7 @@
     </row>
     <row r="7" spans="1:239" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C7" s="35"/>
       <c r="E7"/>
@@ -41404,10 +41365,10 @@
     </row>
     <row r="8" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="16"/>
@@ -41652,10 +41613,10 @@
     </row>
     <row r="9" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="17">
@@ -41908,7 +41869,7 @@
     </row>
     <row r="10" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B10" s="45" t="s">
         <v>17</v>
@@ -42165,7 +42126,7 @@
     <row r="11" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="17"/>
@@ -42414,7 +42375,7 @@
     <row r="12" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32"/>
       <c r="B12" s="45" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="17">
@@ -42919,7 +42880,7 @@
     <row r="14" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32"/>
       <c r="B14" s="45" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C14" s="39"/>
       <c r="D14" s="17">
@@ -43420,10 +43381,10 @@
     </row>
     <row r="16" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="19"/>
@@ -43669,7 +43630,7 @@
     <row r="17" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
       <c r="B17" s="46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="20">
@@ -44177,7 +44138,7 @@
     <row r="19" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32"/>
       <c r="B19" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="20">
@@ -44682,7 +44643,7 @@
     <row r="21" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="32"/>
       <c r="B21" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="20">
@@ -45183,10 +45144,10 @@
     </row>
     <row r="23" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="22"/>
@@ -45432,7 +45393,7 @@
     <row r="24" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32"/>
       <c r="B24" s="47" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="23">
@@ -45940,7 +45901,7 @@
     <row r="26" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="32"/>
       <c r="B26" s="47" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="23">
@@ -46445,7 +46406,7 @@
     <row r="28" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="32"/>
       <c r="B28" s="47" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="23">
@@ -46946,7 +46907,7 @@
     </row>
     <row r="30" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B30" s="48"/>
       <c r="C30" s="44"/>
@@ -47192,10 +47153,10 @@
     </row>
     <row r="31" spans="1:239" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="26"/>
@@ -47450,12 +47411,23 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="HK4:HQ4"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="HY4:IE4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="FG4:FM4"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
     <mergeCell ref="DJ4:DP4"/>
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
@@ -47468,23 +47440,12 @@
     <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="HK4:HQ4"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="HY4:IE4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D31">
     <cfRule type="dataBar" priority="1">
@@ -47553,15 +47514,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="0d1dea18-7b56-4ac7-aa1d-7834839a8030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a9f3451a-73cb-4405-a932-26db050e40a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_Flow_SignoffStatus xmlns="a9f3451a-73cb-4405-a932-26db050e40a8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47832,27 +47790,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="0d1dea18-7b56-4ac7-aa1d-7834839a8030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a9f3451a-73cb-4405-a932-26db050e40a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_Flow_SignoffStatus xmlns="a9f3451a-73cb-4405-a932-26db050e40a8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0d1dea18-7b56-4ac7-aa1d-7834839a8030"/>
-    <ds:schemaRef ds:uri="a9f3451a-73cb-4405-a932-26db050e40a8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -47877,9 +47829,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC3AD2E1-977A-4D4F-8EE8-D64B5FFADF75}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0d1dea18-7b56-4ac7-aa1d-7834839a8030"/>
+    <ds:schemaRef ds:uri="a9f3451a-73cb-4405-a932-26db050e40a8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>